<commit_message>
name for zheng parameter also changed in general info #42
</commit_message>
<xml_diff>
--- a/hackathon_contributions_new_data_format/Zheng_PNAS2012/General_info.xlsx
+++ b/hackathon_contributions_new_data_format/Zheng_PNAS2012/General_info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">log10(k32_31)</t>
   </si>
   <si>
-    <t xml:space="preserve">log10(noise)</t>
+    <t xml:space="preserve">log10(sigma)</t>
   </si>
   <si>
     <t xml:space="preserve">Conditions</t>
@@ -580,6 +580,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -663,7 +664,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -782,8 +783,8 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>